<commit_message>
other foles and text
</commit_message>
<xml_diff>
--- a/backend/python/xlsx/tmp.xlsx
+++ b/backend/python/xlsx/tmp.xlsx
@@ -12,19 +12,16 @@
     <workbookView xWindow="120" yWindow="30" windowWidth="15180" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Αυστρία</t>
-  </si>
-  <si>
-    <t>Βέλγιο</t>
   </si>
   <si>
     <t>Γαλλία</t>
@@ -45,31 +42,10 @@
     <t>Ολλανδία</t>
   </si>
   <si>
-    <t>Δανία</t>
-  </si>
-  <si>
-    <t>Ρουμανία</t>
-  </si>
-  <si>
-    <t>Σουηδία</t>
-  </si>
-  <si>
     <t>Τσεχία</t>
   </si>
   <si>
-    <t>Αλβανία</t>
-  </si>
-  <si>
-    <t>Αυστραλία</t>
-  </si>
-  <si>
-    <t>Ελβετία</t>
-  </si>
-  <si>
     <t>ΗΠΑ</t>
-  </si>
-  <si>
-    <t>Καναδάς</t>
   </si>
   <si>
     <t>Ρωσία</t>
@@ -78,31 +54,37 @@
     <t>ΣΥΝΟΛΟ</t>
   </si>
   <si>
-    <t>Κρουαζιέρες</t>
+    <t>Χώρες_ζώνης_ευρώ</t>
   </si>
   <si>
-    <t>Χώρες_ζώνης_ευρώ</t>
+    <t>Μεμονωμένοι_ταξιδιώτες</t>
+  </si>
+  <si>
+    <t>Ετος</t>
+  </si>
+  <si>
+    <t>Βουλγαρία</t>
+  </si>
+  <si>
+    <t>Ηνωμένο_Βασίλειο</t>
+  </si>
+  <si>
+    <t>Πολωνία</t>
+  </si>
+  <si>
+    <t>Αίγυπτος</t>
+  </si>
+  <si>
+    <t>Τουρκία</t>
+  </si>
+  <si>
+    <t>Οργανωμένα_ταξίδια</t>
   </si>
   <si>
     <t>Χώρες_EE_εκτός_ζώνης_ευρώ</t>
   </si>
   <si>
     <t>Λοιπές_Χώρες</t>
-  </si>
-  <si>
-    <t>Μεμονωμένοι_ταξιδιώτες</t>
-  </si>
-  <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>Ετος</t>
-  </si>
-  <si>
-    <t>Ηνωμένο_Βασίλειο</t>
-  </si>
-  <si>
-    <t>Οργανωμένα_ταξίδια</t>
   </si>
   <si>
     <t>Χώρες_ΕΕ_27</t>
@@ -112,9 +94,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="##,###,##0.0"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -133,20 +116,41 @@
       <charset val="161"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC1C1C1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC1C1C1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC1C1C1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC1C1C1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -155,7 +159,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -167,10 +171,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -488,28 +489,27 @@
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="16.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
@@ -518,14 +518,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="7" t="s">
-        <v>25</v>
+      <c r="A1" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -549,145 +549,123 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" t="s">
-        <v>15</v>
-      </c>
       <c r="W1" t="s">
-        <v>16</v>
-      </c>
-      <c r="X1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="Y1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="6">
         <v>2005</v>
       </c>
       <c r="B2" s="2">
-        <v>729.70212937659949</v>
+        <v>6.6727754907180366</v>
       </c>
       <c r="C2" s="2">
-        <v>788.78225483921165</v>
+        <v>7.6140129164959864</v>
       </c>
       <c r="D2" s="2">
-        <v>714.64874346720023</v>
+        <v>4.7786937832809393</v>
       </c>
       <c r="E2" s="2">
-        <v>770.92353352433963</v>
+        <v>6.9295917865284631</v>
       </c>
       <c r="F2" s="2">
-        <v>819.69913886399092</v>
+        <v>9.3498799344750232</v>
       </c>
       <c r="G2" s="2">
-        <v>803.38966348979056</v>
+        <v>7.5486150337315756</v>
       </c>
       <c r="H2" s="2">
-        <v>899.68342229362077</v>
+        <v>6.0303481943754438</v>
       </c>
       <c r="I2" s="2">
-        <v>779.47743937609766</v>
+        <v>11.969693107384707</v>
       </c>
       <c r="J2" s="2">
-        <v>706.25856513768179</v>
+        <v>5.4093552597233101</v>
       </c>
       <c r="K2" s="2">
-        <v>894.02251846433796</v>
+        <v>4.7689310754724588</v>
       </c>
       <c r="L2" s="2">
-        <v>502.79900276425991</v>
+        <v>3.0359340735628617</v>
       </c>
       <c r="M2" s="2">
-        <v>648.25039500637581</v>
+        <v>7.48770630793579</v>
       </c>
       <c r="N2" s="2">
-        <v>574.39934811471812</v>
+        <v>5.3324260703251438</v>
       </c>
       <c r="O2" s="2">
-        <v>588.30132296794693</v>
+        <v>11.087561834857887</v>
       </c>
       <c r="P2" s="2">
-        <v>546.81497518008064</v>
+        <v>13.479871491274379</v>
       </c>
       <c r="Q2" s="2">
-        <v>771.94968221688896</v>
+        <v>18.677094448743535</v>
       </c>
       <c r="R2" s="2">
-        <v>321.27362245631986</v>
+        <v>24.414533272061547</v>
       </c>
       <c r="S2" s="2">
-        <v>1099.751314558267</v>
+        <v>15.547515110812625</v>
       </c>
       <c r="T2" s="2">
-        <v>892.07401764769725</v>
+        <v>4.8627394954089471</v>
       </c>
       <c r="U2" s="2">
-        <v>845.04838479793364</v>
+        <v>9.3815076564222615</v>
       </c>
       <c r="V2" s="2">
-        <v>1211.3089931540439</v>
+        <v>10.016676388211208</v>
       </c>
       <c r="W2" s="2">
-        <v>1120.4100233119036</v>
-      </c>
-      <c r="X2" s="2">
-        <v>1211.8618105906694</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>745.71617178598376</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>690.0090887229635</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>908.05082797720456</v>
-      </c>
+        <v>5.007663262338566</v>
+      </c>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
     </row>
     <row r="3" spans="1:29">
@@ -695,86 +673,76 @@
         <v>2006</v>
       </c>
       <c r="B3" s="2">
-        <v>725.5226184313525</v>
+        <v>7.0659231056520113</v>
       </c>
       <c r="C3" s="2">
-        <v>776.70039475831175</v>
+        <v>8.1539625366257997</v>
       </c>
       <c r="D3" s="2">
-        <v>694.2924047152145</v>
+        <v>3.8639051321420403</v>
       </c>
       <c r="E3" s="2">
-        <v>782.24371077370188</v>
+        <v>7.1108051312249589</v>
       </c>
       <c r="F3" s="2">
-        <v>749.42112246563715</v>
+        <v>9.0426670220665226</v>
       </c>
       <c r="G3" s="2">
-        <v>852.56812539038503</v>
+        <v>6.8088813750352211</v>
       </c>
       <c r="H3" s="2">
-        <v>791.45931085692064</v>
+        <v>9.5328003105929167</v>
       </c>
       <c r="I3" s="2">
-        <v>669.17095481898434</v>
+        <v>11.96342544047496</v>
       </c>
       <c r="J3" s="2">
-        <v>688.49037417398563</v>
+        <v>5.9192500430436867</v>
       </c>
       <c r="K3" s="2">
-        <v>898.08558628212256</v>
+        <v>4.7999469255698131</v>
       </c>
       <c r="L3" s="2">
-        <v>522.98927159121513</v>
+        <v>3.211327132551038</v>
       </c>
       <c r="M3" s="2">
-        <v>685.27785401866959</v>
+        <v>8.8309258646671811</v>
       </c>
       <c r="N3" s="2">
-        <v>572.22722501312137</v>
+        <v>3.9649104846243426</v>
       </c>
       <c r="O3" s="2">
-        <v>622.99201477788608</v>
+        <v>11.375736475629353</v>
       </c>
       <c r="P3" s="2">
-        <v>556.86702582643886</v>
+        <v>10.513628506847494</v>
       </c>
       <c r="Q3" s="2">
-        <v>779.92913650918263</v>
+        <v>16.765007835369918</v>
       </c>
       <c r="R3" s="2">
-        <v>341.51274444793449</v>
+        <v>23.383350954866849</v>
       </c>
       <c r="S3" s="2">
-        <v>1235.3176308268453</v>
+        <v>17.037383614841154</v>
       </c>
       <c r="T3" s="2">
-        <v>831.94816769567819</v>
+        <v>5.5161622925901126</v>
       </c>
       <c r="U3" s="2">
-        <v>842.17447813176432</v>
+        <v>9.7112334292610605</v>
       </c>
       <c r="V3" s="2">
-        <v>1237.5912982031093</v>
+        <v>10.241967268853299</v>
       </c>
       <c r="W3" s="2">
-        <v>1134.7136619597529</v>
-      </c>
-      <c r="X3" s="2">
-        <v>1142.5716400062731</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z3" s="2">
-        <v>745.85808874297993</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>689.94829023618877</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>913.02004380744836</v>
-      </c>
+        <v>5.404607994673257</v>
+      </c>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
     </row>
     <row r="4" spans="1:29">
@@ -782,86 +750,76 @@
         <v>2007</v>
       </c>
       <c r="B4" s="2">
-        <v>682.835014601181</v>
+        <v>6.980289767255651</v>
       </c>
       <c r="C4" s="2">
-        <v>754.40428161345199</v>
+        <v>7.8385315182268709</v>
       </c>
       <c r="D4" s="2">
-        <v>643.63365237355322</v>
+        <v>4.5799093240953708</v>
       </c>
       <c r="E4" s="2">
-        <v>774.46998189231465</v>
+        <v>6.3671170565684703</v>
       </c>
       <c r="F4" s="2">
-        <v>766.27401434666956</v>
+        <v>8.8239557057814544</v>
       </c>
       <c r="G4" s="2">
-        <v>794.46685415532352</v>
+        <v>8.3705604842298911</v>
       </c>
       <c r="H4" s="2">
-        <v>611.44177327716147</v>
+        <v>6.4748237371214845</v>
       </c>
       <c r="I4" s="2">
-        <v>725.11136562851812</v>
+        <v>13.778773894008895</v>
       </c>
       <c r="J4" s="2">
-        <v>672.73541508643473</v>
+        <v>8.6487845384531159</v>
       </c>
       <c r="K4" s="2">
-        <v>891.87423701555815</v>
+        <v>5.0365887433164147</v>
       </c>
       <c r="L4" s="2">
-        <v>452.49349002437651</v>
+        <v>2.7432398235847009</v>
       </c>
       <c r="M4" s="2">
-        <v>691.83580299497851</v>
+        <v>9.2643519041699633</v>
       </c>
       <c r="N4" s="2">
-        <v>520.55810202495638</v>
+        <v>4.2884383574224803</v>
       </c>
       <c r="O4" s="2">
-        <v>567.17968406486818</v>
+        <v>8.7437717948117548</v>
       </c>
       <c r="P4" s="2">
-        <v>539.13661495639542</v>
+        <v>8.7465859945887221</v>
       </c>
       <c r="Q4" s="2">
-        <v>725.80962601310671</v>
+        <v>14.814541737972998</v>
       </c>
       <c r="R4" s="2">
-        <v>321.34796791721544</v>
+        <v>18.228449164776244</v>
       </c>
       <c r="S4" s="2">
-        <v>1036.0433563608451</v>
+        <v>15.855197100339945</v>
       </c>
       <c r="T4" s="2">
-        <v>836.46338663890378</v>
+        <v>6.0029975427422579</v>
       </c>
       <c r="U4" s="2">
-        <v>861.51662540239147</v>
+        <v>9.0461919611061017</v>
       </c>
       <c r="V4" s="2">
-        <v>1228.6444781518944</v>
+        <v>9.4196548349630316</v>
       </c>
       <c r="W4" s="2">
-        <v>1274.7777020745514</v>
-      </c>
-      <c r="X4" s="2">
-        <v>1191.2853986402192</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>700.21679421896272</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>622.38508014186789</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>904.93599338552065</v>
-      </c>
+        <v>5.8997648483030511</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
     </row>
     <row r="5" spans="1:29">
@@ -869,86 +827,76 @@
         <v>2008</v>
       </c>
       <c r="B5" s="2">
-        <v>727.97369302450727</v>
+        <v>7.4333814455389788</v>
       </c>
       <c r="C5" s="2">
-        <v>804.1817241145435</v>
+        <v>8.2771036616234781</v>
       </c>
       <c r="D5" s="2">
-        <v>784.90023795665422</v>
+        <v>4.638276152856065</v>
       </c>
       <c r="E5" s="2">
-        <v>864.40602847112007</v>
+        <v>8.1636538832144918</v>
       </c>
       <c r="F5" s="2">
-        <v>863.22608366764973</v>
+        <v>8.7144351257458972</v>
       </c>
       <c r="G5" s="2">
-        <v>821.02701011647275</v>
+        <v>9.488811949747749</v>
       </c>
       <c r="H5" s="2">
-        <v>645.14146355067214</v>
+        <v>7.5603119028741563</v>
       </c>
       <c r="I5" s="2">
-        <v>755.52364478481184</v>
+        <v>12.261792889382484</v>
       </c>
       <c r="J5" s="2">
-        <v>780.14580785979365</v>
+        <v>7.5476069246435848</v>
       </c>
       <c r="K5" s="2">
-        <v>830.02431244236141</v>
+        <v>5.4985075411521436</v>
       </c>
       <c r="L5" s="2">
-        <v>487.97105028752719</v>
+        <v>2.7229148163709969</v>
       </c>
       <c r="M5" s="2">
-        <v>644.65650056109416</v>
+        <v>11.027687630941132</v>
       </c>
       <c r="N5" s="2">
-        <v>524.61990805363109</v>
+        <v>6.5724288569082772</v>
       </c>
       <c r="O5" s="2">
-        <v>605.93671560072175</v>
+        <v>10.205538549715843</v>
       </c>
       <c r="P5" s="2">
-        <v>682.26887476803688</v>
+        <v>8.0171835632329742</v>
       </c>
       <c r="Q5" s="2">
-        <v>732.88764253489876</v>
+        <v>13.976498262003497</v>
       </c>
       <c r="R5" s="2">
-        <v>367.53734301348186</v>
+        <v>17.776180863022184</v>
       </c>
       <c r="S5" s="2">
-        <v>1186.906265719781</v>
+        <v>14.862144276401136</v>
       </c>
       <c r="T5" s="2">
-        <v>831.78523292428122</v>
+        <v>5.1290206962022253</v>
       </c>
       <c r="U5" s="2">
-        <v>825.20047807709716</v>
+        <v>9.5301368091049898</v>
       </c>
       <c r="V5" s="2">
-        <v>1184.8705242116428</v>
+        <v>10.025379665853237</v>
       </c>
       <c r="W5" s="2">
-        <v>1178.9810852771886</v>
-      </c>
-      <c r="X5" s="2">
-        <v>1295.6874061707304</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>730.03688418693343</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>650.10416341853477</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>920.56728386612087</v>
-      </c>
+        <v>5.6650361344858142</v>
+      </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
     </row>
     <row r="6" spans="1:29">
@@ -956,86 +904,76 @@
         <v>2009</v>
       </c>
       <c r="B6" s="2">
-        <v>709.70405176335305</v>
+        <v>7.4493047379237582</v>
       </c>
       <c r="C6" s="2">
-        <v>787.3702567441544</v>
+        <v>8.2689865468914157</v>
       </c>
       <c r="D6" s="2">
-        <v>811.76911621350473</v>
+        <v>4.3534345253408802</v>
       </c>
       <c r="E6" s="2">
-        <v>938.47556688477403</v>
+        <v>8.8803106695336247</v>
       </c>
       <c r="F6" s="2">
-        <v>783.10685275170886</v>
+        <v>8.5460164343461393</v>
       </c>
       <c r="G6" s="2">
-        <v>808.96321178378878</v>
+        <v>6.9660909418025492</v>
       </c>
       <c r="H6" s="2">
-        <v>665.94055125531281</v>
+        <v>7.7819546849655552</v>
       </c>
       <c r="I6" s="2">
-        <v>702.10483480542314</v>
+        <v>11.747205710594484</v>
       </c>
       <c r="J6" s="2">
-        <v>761.39400732767047</v>
+        <v>7.7687928536387805</v>
       </c>
       <c r="K6" s="2">
-        <v>874.56429861182994</v>
+        <v>5.5669064480464199</v>
       </c>
       <c r="L6" s="2">
-        <v>473.13667739302031</v>
+        <v>2.963406569382959</v>
       </c>
       <c r="M6" s="2">
-        <v>704.19347520631425</v>
+        <v>11.692157510587812</v>
       </c>
       <c r="N6" s="2">
-        <v>557.57696125791426</v>
+        <v>6.919500978137763</v>
       </c>
       <c r="O6" s="2">
-        <v>631.57691429409124</v>
+        <v>9.06084979641372</v>
       </c>
       <c r="P6" s="2">
-        <v>584.28017180205416</v>
+        <v>15.360477399507033</v>
       </c>
       <c r="Q6" s="2">
-        <v>680.50631231101386</v>
+        <v>15.507451681726907</v>
       </c>
       <c r="R6" s="2">
-        <v>384.37237007789992</v>
+        <v>20.336552611077447</v>
       </c>
       <c r="S6" s="2">
-        <v>1354.2780250880182</v>
+        <v>14.037997339460636</v>
       </c>
       <c r="T6" s="2">
-        <v>861.58611171786572</v>
+        <v>4.4952658053062429</v>
       </c>
       <c r="U6" s="2">
-        <v>778.66501135311819</v>
+        <v>9.0662807938164391</v>
       </c>
       <c r="V6" s="2">
-        <v>1076.7302149139928</v>
+        <v>9.3887649607678885</v>
       </c>
       <c r="W6" s="2">
-        <v>1071.318184515861</v>
-      </c>
-      <c r="X6" s="2">
-        <v>1102.3156250685824</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>697.32030636928869</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>620.39473140185373</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>889.86681725633264</v>
-      </c>
+        <v>5.9413355433310642</v>
+      </c>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
     </row>
     <row r="7" spans="1:29">
@@ -1043,86 +981,76 @@
         <v>2010</v>
       </c>
       <c r="B7" s="2">
-        <v>649.74312556662971</v>
+        <v>6.618049275136852</v>
       </c>
       <c r="C7" s="2">
-        <v>740.83473122251826</v>
+        <v>7.4554757809359469</v>
       </c>
       <c r="D7" s="2">
-        <v>816.55265141104189</v>
+        <v>4.376016359121671</v>
       </c>
       <c r="E7" s="2">
-        <v>727.971468590732</v>
+        <v>6.3884936358327424</v>
       </c>
       <c r="F7" s="2">
-        <v>738.4218723368972</v>
+        <v>7.778933019498937</v>
       </c>
       <c r="G7" s="2">
-        <v>796.45817147913158</v>
+        <v>6.9490028890788489</v>
       </c>
       <c r="H7" s="2">
-        <v>644.52817091859731</v>
+        <v>6.7112750083811106</v>
       </c>
       <c r="I7" s="2">
-        <v>641.88239484786232</v>
+        <v>10.995269990793494</v>
       </c>
       <c r="J7" s="2">
-        <v>653.03662540376172</v>
+        <v>7.2301265304648279</v>
       </c>
       <c r="K7" s="2">
-        <v>840.72940894001715</v>
+        <v>4.7934058862609223</v>
       </c>
       <c r="L7" s="2">
-        <v>402.29015303633417</v>
+        <v>2.0790294142341383</v>
       </c>
       <c r="M7" s="2">
-        <v>572.10993793725549</v>
+        <v>8.3499798020601901</v>
       </c>
       <c r="N7" s="2">
-        <v>417.2739075990246</v>
+        <v>7.0783585582774222</v>
       </c>
       <c r="O7" s="2">
-        <v>537.67495285871848</v>
+        <v>8.1414907986093308</v>
       </c>
       <c r="P7" s="2">
-        <v>543.44546274445986</v>
+        <v>6.746536460093262</v>
       </c>
       <c r="Q7" s="2">
-        <v>628.55959162154784</v>
+        <v>12.415003241841365</v>
       </c>
       <c r="R7" s="2">
-        <v>323.0840658614365</v>
+        <v>17.712424731815315</v>
       </c>
       <c r="S7" s="2">
-        <v>1357.0589612167864</v>
+        <v>16.159418820746748</v>
       </c>
       <c r="T7" s="2">
-        <v>965.6834220662563</v>
+        <v>4.0209012529596766</v>
       </c>
       <c r="U7" s="2">
-        <v>690.40753700195648</v>
+        <v>8.2509835856738132</v>
       </c>
       <c r="V7" s="2">
-        <v>1202.0032370188121</v>
+        <v>8.6652844023159812</v>
       </c>
       <c r="W7" s="2">
-        <v>1185.1018101942518</v>
-      </c>
-      <c r="X7" s="2">
-        <v>1099.0668980296473</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>640.43123351781674</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>583.94858486900807</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>795.37970215967982</v>
-      </c>
+        <v>5.5361105103118362</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
     </row>
     <row r="8" spans="1:29">
@@ -1130,86 +1058,76 @@
         <v>2011</v>
       </c>
       <c r="B8" s="2">
-        <v>657.50603739060421</v>
+        <v>6.2329017439945389</v>
       </c>
       <c r="C8" s="2">
-        <v>751.3638908072993</v>
+        <v>7.6485050117945246</v>
       </c>
       <c r="D8" s="2">
-        <v>822.94516837109541</v>
+        <v>3.2540816683578853</v>
       </c>
       <c r="E8" s="2">
-        <v>731.16197754045447</v>
+        <v>7.3704082430907123</v>
       </c>
       <c r="F8" s="2">
-        <v>730.50847075532249</v>
+        <v>7.3012267270450364</v>
       </c>
       <c r="G8" s="2">
-        <v>820.48727420656576</v>
+        <v>9.4371482324047324</v>
       </c>
       <c r="H8" s="2">
-        <v>871.70227312298039</v>
+        <v>5.7368692702828916</v>
       </c>
       <c r="I8" s="2">
-        <v>668.20971280176639</v>
+        <v>14.662268712631912</v>
       </c>
       <c r="J8" s="2">
-        <v>686.88387611412452</v>
+        <v>6.0161247066711363</v>
       </c>
       <c r="K8" s="2">
-        <v>750.68851732996791</v>
+        <v>3.7566024553553135</v>
       </c>
       <c r="L8" s="2">
-        <v>392.69692071117481</v>
+        <v>2.0379629513264881</v>
       </c>
       <c r="M8" s="2">
-        <v>588.14113353640073</v>
+        <v>9.270844837106571</v>
       </c>
       <c r="N8" s="2">
-        <v>319.04852256006092</v>
+        <v>4.4513045315305799</v>
       </c>
       <c r="O8" s="2">
-        <v>563.9830597850206</v>
+        <v>5.8036381695434498</v>
       </c>
       <c r="P8" s="2">
-        <v>534.93768397835413</v>
+        <v>12.429141531322506</v>
       </c>
       <c r="Q8" s="2">
-        <v>617.78193596409687</v>
+        <v>12.560754262455092</v>
       </c>
       <c r="R8" s="2">
-        <v>297.39221909272862</v>
+        <v>16.932803506086373</v>
       </c>
       <c r="S8" s="2">
-        <v>1420.3774806541348</v>
+        <v>14.626037190328137</v>
       </c>
       <c r="T8" s="2">
-        <v>966.59482069876344</v>
+        <v>4.0942707865056294</v>
       </c>
       <c r="U8" s="2">
-        <v>685.62561157747837</v>
+        <v>6.7633572330597804</v>
       </c>
       <c r="V8" s="2">
-        <v>1098.557307501512</v>
+        <v>6.9437513883047828</v>
       </c>
       <c r="W8" s="2">
-        <v>1207.073307097422</v>
-      </c>
-      <c r="X8" s="2">
-        <v>1005.4613730339361</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>639.46977388503672</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>582.23462016376232</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>792.15887485907319</v>
-      </c>
+        <v>5.1411726332592487</v>
+      </c>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
     </row>
     <row r="9" spans="1:29">
@@ -1217,86 +1135,76 @@
         <v>2012</v>
       </c>
       <c r="B9" s="2">
-        <v>653.23678336749344</v>
+        <v>7.7299693924019275</v>
       </c>
       <c r="C9" s="2">
-        <v>735.18432526866559</v>
+        <v>9.5915471391601166</v>
       </c>
       <c r="D9" s="2">
-        <v>822.59393783018993</v>
+        <v>5.3154515433140102</v>
       </c>
       <c r="E9" s="2">
-        <v>794.87192372865809</v>
+        <v>7.7271309511927342</v>
       </c>
       <c r="F9" s="2">
-        <v>781.57355569765957</v>
+        <v>9.4973983260045056</v>
       </c>
       <c r="G9" s="2">
-        <v>784.47508069805053</v>
+        <v>10.378718845592886</v>
       </c>
       <c r="H9" s="2">
-        <v>713.8713476580059</v>
+        <v>7.2610848454987966</v>
       </c>
       <c r="I9" s="2">
-        <v>640.40988452645001</v>
+        <v>16.483439261068881</v>
       </c>
       <c r="J9" s="2">
-        <v>658.42255299049907</v>
+        <v>8.4382833911337976</v>
       </c>
       <c r="K9" s="2">
-        <v>652.8917441688028</v>
+        <v>3.9363202335594378</v>
       </c>
       <c r="L9" s="2">
-        <v>408.83691896520799</v>
+        <v>2.5677772410786868</v>
       </c>
       <c r="M9" s="2">
-        <v>636.8572229207482</v>
+        <v>9.2770488756736658</v>
       </c>
       <c r="N9" s="2">
-        <v>415.61960711123459</v>
+        <v>4.0560416352391009</v>
       </c>
       <c r="O9" s="2">
-        <v>595.83263175671448</v>
+        <v>6.5771268509736043</v>
       </c>
       <c r="P9" s="2">
-        <v>514.27060988942549</v>
+        <v>14.446399917179978</v>
       </c>
       <c r="Q9" s="2">
-        <v>638.59917692558406</v>
+        <v>15.730605063373627</v>
       </c>
       <c r="R9" s="2">
-        <v>313.98047803245845</v>
+        <v>20.175662085149177</v>
       </c>
       <c r="S9" s="2">
-        <v>1327.2904041475397</v>
+        <v>17.352685706905181</v>
       </c>
       <c r="T9" s="2">
-        <v>990.99658567518861</v>
+        <v>3.7873923353046477</v>
       </c>
       <c r="U9" s="2">
-        <v>739.01435604234496</v>
+        <v>7.6974879697328191</v>
       </c>
       <c r="V9" s="2">
-        <v>1139.3493440903935</v>
+        <v>7.8638276755793193</v>
       </c>
       <c r="W9" s="2">
-        <v>1281.259021948702</v>
-      </c>
-      <c r="X9" s="2">
-        <v>1079.0306611780925</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>292.21598394872774</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>616.20089738893523</v>
-      </c>
-      <c r="AA9" s="2">
-        <v>578.90818978656864</v>
-      </c>
-      <c r="AB9" s="2">
-        <v>692.77125597761653</v>
-      </c>
+        <v>5.3738774560071478</v>
+      </c>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
     </row>
     <row r="10" spans="1:29">
@@ -1304,86 +1212,76 @@
         <v>2013</v>
       </c>
       <c r="B10" s="2">
-        <v>671.08262493333007</v>
+        <v>7.6228936934704494</v>
       </c>
       <c r="C10" s="2">
-        <v>762.06407675981052</v>
+        <v>9.5576416872188279</v>
       </c>
       <c r="D10" s="2">
-        <v>898.13177658620748</v>
+        <v>5.0138231453521582</v>
       </c>
       <c r="E10" s="2">
-        <v>822.05670825678487</v>
+        <v>8.8664634879897335</v>
       </c>
       <c r="F10" s="2">
-        <v>785.87164310195044</v>
+        <v>10.880116434786993</v>
       </c>
       <c r="G10" s="2">
-        <v>838.06690936673806</v>
+        <v>11.115793954874414</v>
       </c>
       <c r="H10" s="2">
-        <v>755.81102969952599</v>
+        <v>6.484676361268443</v>
       </c>
       <c r="I10" s="2">
-        <v>622.66228738771815</v>
+        <v>15.244395687061184</v>
       </c>
       <c r="J10" s="2">
-        <v>617.80505702878884</v>
+        <v>10.556586518078857</v>
       </c>
       <c r="K10" s="2">
-        <v>706.28985587086913</v>
+        <v>4.312757389668973</v>
       </c>
       <c r="L10" s="2">
-        <v>418.8915044863021</v>
+        <v>2.2656325856879307</v>
       </c>
       <c r="M10" s="2">
-        <v>574.90988561607298</v>
+        <v>10.311378196643194</v>
       </c>
       <c r="N10" s="2">
-        <v>434.96019707825042</v>
+        <v>10.023499672315326</v>
       </c>
       <c r="O10" s="2">
-        <v>615.26998866698841</v>
+        <v>6.5302420361871656</v>
       </c>
       <c r="P10" s="2">
-        <v>532.0161687121481</v>
+        <v>20.860107127346428</v>
       </c>
       <c r="Q10" s="2">
-        <v>636.60743651870075</v>
+        <v>19.087812486826021</v>
       </c>
       <c r="R10" s="2">
-        <v>330.5645116559167</v>
+        <v>24.718803835527385</v>
       </c>
       <c r="S10" s="2">
-        <v>1369.5889583381741</v>
+        <v>18.71410833750301</v>
       </c>
       <c r="T10" s="2">
-        <v>961.30419286788242</v>
+        <v>4.5768342847548693</v>
       </c>
       <c r="U10" s="2">
-        <v>733.73834175002116</v>
+        <v>7.7288566875477516</v>
       </c>
       <c r="V10" s="2">
-        <v>1218.791451599074</v>
+        <v>7.8779443255820656</v>
       </c>
       <c r="W10" s="2">
-        <v>1388.2613390465988</v>
-      </c>
-      <c r="X10" s="2">
-        <v>989.39438288537008</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>203.12978413261825</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>604.24535718930201</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>582.58602437226693</v>
-      </c>
-      <c r="AB10" s="2">
-        <v>645.05809411178575</v>
-      </c>
+        <v>5.7574888885242759</v>
+      </c>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
     <row r="11" spans="1:29">
@@ -1391,86 +1289,76 @@
         <v>2014</v>
       </c>
       <c r="B11" s="2">
-        <v>599.48413553440832</v>
+        <v>7.0649388845591314</v>
       </c>
       <c r="C11" s="2">
-        <v>731.08059788083904</v>
+        <v>9.2717086726545563</v>
       </c>
       <c r="D11" s="2">
-        <v>860.65695066478213</v>
+        <v>3.8357413647851728</v>
       </c>
       <c r="E11" s="2">
-        <v>762.06700651761128</v>
+        <v>7.4969159806873398</v>
       </c>
       <c r="F11" s="2">
-        <v>771.66516762703168</v>
+        <v>9.1399631440198608</v>
       </c>
       <c r="G11" s="2">
-        <v>811.02747447572983</v>
+        <v>9.1549599342730019</v>
       </c>
       <c r="H11" s="2">
-        <v>569.84893929384134</v>
+        <v>7.1583178069430362</v>
       </c>
       <c r="I11" s="2">
-        <v>629.98276924893821</v>
+        <v>19.044272742990348</v>
       </c>
       <c r="J11" s="2">
-        <v>569.5160067180708</v>
+        <v>10.556524492407551</v>
       </c>
       <c r="K11" s="2">
-        <v>661.17576927582263</v>
+        <v>3.8853986774130718</v>
       </c>
       <c r="L11" s="2">
-        <v>334.5242516008916</v>
+        <v>2.1065036729538971</v>
       </c>
       <c r="M11" s="2">
-        <v>610.32015073746561</v>
+        <v>8.4861633642672025</v>
       </c>
       <c r="N11" s="2">
-        <v>345.61831636793954</v>
+        <v>7.3337492406954405</v>
       </c>
       <c r="O11" s="2">
-        <v>594.3877946170312</v>
+        <v>6.2114320627824915</v>
       </c>
       <c r="P11" s="2">
-        <v>451.70192794513611</v>
+        <v>14.261837359910032</v>
       </c>
       <c r="Q11" s="2">
-        <v>580.75308091039108</v>
+        <v>18.253152883980508</v>
       </c>
       <c r="R11" s="2">
-        <v>293.48862523509621</v>
+        <v>23.785602775368602</v>
       </c>
       <c r="S11" s="2">
-        <v>1304.9940245028156</v>
+        <v>19.895677132146204</v>
       </c>
       <c r="T11" s="2">
-        <v>896.05687978020342</v>
+        <v>3.7899184324269184</v>
       </c>
       <c r="U11" s="2">
-        <v>743.10163917322996</v>
+        <v>7.1982716568292773</v>
       </c>
       <c r="V11" s="2">
-        <v>1106.811213257346</v>
+        <v>7.2780946477817663</v>
       </c>
       <c r="W11" s="2">
-        <v>1125.3201528949157</v>
-      </c>
-      <c r="X11" s="2">
-        <v>925.18905928294782</v>
-      </c>
-      <c r="Y11" s="2">
-        <v>173.28375189420993</v>
-      </c>
-      <c r="Z11" s="2">
-        <v>551.77961450113821</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>526.62919201424199</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>609.97913021230511</v>
-      </c>
+        <v>6.0046030998403301</v>
+      </c>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
     <row r="12" spans="1:29">
@@ -1478,86 +1366,76 @@
         <v>2015</v>
       </c>
       <c r="B12" s="2">
-        <v>587.08842136146507</v>
+        <v>6.2633458494832039</v>
       </c>
       <c r="C12" s="2">
-        <v>733.70566991539408</v>
+        <v>9.2498018522022516</v>
       </c>
       <c r="D12" s="2">
-        <v>918.60279529593026</v>
+        <v>4.6387546805169704</v>
       </c>
       <c r="E12" s="2">
-        <v>773.32065140801285</v>
+        <v>8.5670690079881755</v>
       </c>
       <c r="F12" s="2">
-        <v>784.62026607975827</v>
+        <v>10.190782170395336</v>
       </c>
       <c r="G12" s="2">
-        <v>798.70690366214308</v>
+        <v>9.1853509384455876</v>
       </c>
       <c r="H12" s="2">
-        <v>709.70040481505612</v>
+        <v>7.8649178761514493</v>
       </c>
       <c r="I12" s="2">
-        <v>614.40313311380487</v>
+        <v>14.100048144017649</v>
       </c>
       <c r="J12" s="2">
-        <v>530.06522978480803</v>
+        <v>11.97984151781513</v>
       </c>
       <c r="K12" s="2">
-        <v>686.52706823740004</v>
+        <v>3.1729510317924339</v>
       </c>
       <c r="L12" s="2">
-        <v>313.44527417269137</v>
+        <v>1.9929219530360314</v>
       </c>
       <c r="M12" s="2">
-        <v>598.25215437438987</v>
+        <v>10.026579419769529</v>
       </c>
       <c r="N12" s="2">
-        <v>331.30368376924201</v>
+        <v>5.0754830399313011</v>
       </c>
       <c r="O12" s="2">
-        <v>627.67708555548916</v>
+        <v>5.9159235872164073</v>
       </c>
       <c r="P12" s="2">
-        <v>461.63103154539459</v>
+        <v>11.534323197396523</v>
       </c>
       <c r="Q12" s="2">
-        <v>571.14166180421614</v>
+        <v>16.922825395416279</v>
       </c>
       <c r="R12" s="2">
-        <v>298.92374944035168</v>
+        <v>25.886417616720955</v>
       </c>
       <c r="S12" s="2">
-        <v>1295.0096525518115</v>
+        <v>16.989126676808187</v>
       </c>
       <c r="T12" s="2">
-        <v>957.86790697436663</v>
+        <v>3.856275396764548</v>
       </c>
       <c r="U12" s="2">
-        <v>842.43394645934438</v>
+        <v>6.4343561854155178</v>
       </c>
       <c r="V12" s="2">
-        <v>1257.3626519658087</v>
+        <v>6.4079747814355708</v>
       </c>
       <c r="W12" s="2">
-        <v>1221.7120774112859</v>
-      </c>
-      <c r="X12" s="2">
-        <v>821.58414084545495</v>
-      </c>
-      <c r="Y12" s="2">
-        <v>177.59777341943985</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>540.92400038362473</v>
-      </c>
-      <c r="AA12" s="2">
-        <v>521.67942326766536</v>
-      </c>
-      <c r="AB12" s="2">
-        <v>590.35111005771648</v>
-      </c>
+        <v>6.8409996274174807</v>
+      </c>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
     <row r="13" spans="1:29">
@@ -1565,86 +1443,76 @@
         <v>2016</v>
       </c>
       <c r="B13" s="2">
-        <v>499.45121927548252</v>
+        <v>5.4672942591289786</v>
       </c>
       <c r="C13" s="2">
-        <v>624.55653518222823</v>
+        <v>8.4833807402949848</v>
       </c>
       <c r="D13" s="2">
-        <v>699.93222132494225</v>
+        <v>4.1242845924741607</v>
       </c>
       <c r="E13" s="2">
-        <v>679.90530629022112</v>
+        <v>8.8256585536050043</v>
       </c>
       <c r="F13" s="2">
-        <v>676.66828773630868</v>
+        <v>9.3133042279411757</v>
       </c>
       <c r="G13" s="2">
-        <v>677.95789004168876</v>
+        <v>8.9271311063721175</v>
       </c>
       <c r="H13" s="2">
-        <v>636.07697378129762</v>
+        <v>7.0976974534021515</v>
       </c>
       <c r="I13" s="2">
-        <v>520.70191044500621</v>
+        <v>13.798117170771899</v>
       </c>
       <c r="J13" s="2">
-        <v>476.18758857633668</v>
+        <v>7.1915335169880628</v>
       </c>
       <c r="K13" s="2">
-        <v>623.69816009030865</v>
+        <v>2.8199275152767109</v>
       </c>
       <c r="L13" s="2">
-        <v>291.96093996385184</v>
+        <v>1.5223743787749637</v>
       </c>
       <c r="M13" s="2">
-        <v>549.31165881248012</v>
+        <v>10.788051118210863</v>
       </c>
       <c r="N13" s="2">
-        <v>381.29819512527899</v>
+        <v>3.8674865412159827</v>
       </c>
       <c r="O13" s="2">
-        <v>535.59067274734207</v>
+        <v>5.1846785852459183</v>
       </c>
       <c r="P13" s="2">
-        <v>439.18960799911531</v>
+        <v>14.475029954469207</v>
       </c>
       <c r="Q13" s="2">
-        <v>534.11811086172838</v>
+        <v>14.248437085590876</v>
       </c>
       <c r="R13" s="2">
-        <v>235.64404642090298</v>
+        <v>19.789972746656876</v>
       </c>
       <c r="S13" s="2">
-        <v>1075.5999066017214</v>
+        <v>13.053023702947096</v>
       </c>
       <c r="T13" s="2">
-        <v>767.67328413064979</v>
+        <v>3.0252265204245243</v>
       </c>
       <c r="U13" s="2">
-        <v>671.65084405568189</v>
+        <v>5.6789165922538443</v>
       </c>
       <c r="V13" s="2">
-        <v>934.86646639987259</v>
+        <v>5.6639147524139606</v>
       </c>
       <c r="W13" s="2">
-        <v>925.33676013480351</v>
-      </c>
-      <c r="X13" s="2">
-        <v>732.29034294907319</v>
-      </c>
-      <c r="Y13" s="2">
-        <v>139.84598570553629</v>
-      </c>
-      <c r="Z13" s="2">
-        <v>470.48050417057175</v>
-      </c>
-      <c r="AA13" s="2">
-        <v>462.56774622449967</v>
-      </c>
-      <c r="AB13" s="2">
-        <v>488.21924012508782</v>
-      </c>
+        <v>5.9043690489457292</v>
+      </c>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
     <row r="14" spans="1:29">
@@ -1652,86 +1520,76 @@
         <v>2017</v>
       </c>
       <c r="B14" s="2">
-        <v>501.08282816043084</v>
+        <v>5.0810000856443684</v>
       </c>
       <c r="C14" s="2">
-        <v>638.32436302613428</v>
+        <v>9.4053476069286681</v>
       </c>
       <c r="D14" s="2">
-        <v>648.79204071838137</v>
+        <v>4.5624673850919848</v>
       </c>
       <c r="E14" s="2">
-        <v>648.38761999715143</v>
+        <v>10.31560963751283</v>
       </c>
       <c r="F14" s="2">
-        <v>699.99625932966569</v>
+        <v>10.076577914778223</v>
       </c>
       <c r="G14" s="2">
-        <v>688.8097980274963</v>
+        <v>15.029226751030018</v>
       </c>
       <c r="H14" s="2">
-        <v>535.119721444731</v>
+        <v>6.4456093243601478</v>
       </c>
       <c r="I14" s="2">
-        <v>522.67245219239885</v>
+        <v>13.958466617549684</v>
       </c>
       <c r="J14" s="2">
-        <v>528.34783744130061</v>
+        <v>9.1527086798317931</v>
       </c>
       <c r="K14" s="2">
-        <v>675.73350197802063</v>
+        <v>2.1391590195338916</v>
       </c>
       <c r="L14" s="2">
-        <v>264.32981315804341</v>
+        <v>1.3625994668267041</v>
       </c>
       <c r="M14" s="2">
-        <v>525.39357619666987</v>
+        <v>9.9790249114322673</v>
       </c>
       <c r="N14" s="2">
-        <v>325.82584529794315</v>
+        <v>6.5152355396541441</v>
       </c>
       <c r="O14" s="2">
-        <v>550.66369387246311</v>
+        <v>5.4831840348191214</v>
       </c>
       <c r="P14" s="2">
-        <v>389.60731353749873</v>
+        <v>17.427076826983136</v>
       </c>
       <c r="Q14" s="2">
-        <v>550.67485288592889</v>
+        <v>14.42385358004827</v>
       </c>
       <c r="R14" s="2">
-        <v>229.26691489823793</v>
+        <v>21.771740234789917</v>
       </c>
       <c r="S14" s="2">
-        <v>1218.4291373443125</v>
+        <v>13.507336363311026</v>
       </c>
       <c r="T14" s="2">
-        <v>760.28533051776219</v>
+        <v>2.882328173772176</v>
       </c>
       <c r="U14" s="2">
-        <v>687.75686449423426</v>
+        <v>5.4905977416988074</v>
       </c>
       <c r="V14" s="2">
-        <v>941.06704080488271</v>
+        <v>5.4727949202826416</v>
       </c>
       <c r="W14" s="2">
-        <v>903.01265931490173</v>
-      </c>
-      <c r="X14" s="2">
-        <v>710.32784069771196</v>
-      </c>
-      <c r="Y14" s="2">
-        <v>144.14549495169524</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>485.06693391073645</v>
-      </c>
-      <c r="AA14" s="2">
-        <v>472.59429995338553</v>
-      </c>
-      <c r="AB14" s="2">
-        <v>510.28138558440895</v>
-      </c>
+        <v>5.7191823807065267</v>
+      </c>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
     </row>
     <row r="15" spans="1:29">
@@ -1739,430 +1597,380 @@
         <v>2018</v>
       </c>
       <c r="B15" s="2">
-        <v>491.55054963073474</v>
+        <v>5.1516921400324778</v>
       </c>
       <c r="C15" s="2">
-        <v>621.01193151119855</v>
+        <v>9.4855736579518339</v>
       </c>
       <c r="D15" s="2">
-        <v>698.00129988825188</v>
+        <v>4.6615167262903077</v>
       </c>
       <c r="E15" s="2">
-        <v>680.71232643209498</v>
+        <v>10.603902896305739</v>
       </c>
       <c r="F15" s="2">
-        <v>626.08141267623841</v>
+        <v>11.317203364896754</v>
       </c>
       <c r="G15" s="2">
-        <v>675.93705186048078</v>
+        <v>8.809544800512338</v>
       </c>
       <c r="H15" s="2">
-        <v>545.03007721990616</v>
+        <v>5.7590871377491553</v>
       </c>
       <c r="I15" s="2">
-        <v>563.18153647560996</v>
+        <v>14.842771112642525</v>
       </c>
       <c r="J15" s="2">
-        <v>517.38128667705848</v>
+        <v>7.7507121398440297</v>
       </c>
       <c r="K15" s="2">
-        <v>606.34483811790767</v>
+        <v>2.1254079486445567</v>
       </c>
       <c r="L15" s="2">
-        <v>280.59148086114686</v>
+        <v>1.3443726485921077</v>
       </c>
       <c r="M15" s="2">
-        <v>554.29440920781292</v>
+        <v>10.089593444467891</v>
       </c>
       <c r="N15" s="2">
-        <v>323.89033020056166</v>
+        <v>7.2614644033443119</v>
       </c>
       <c r="O15" s="2">
-        <v>547.47954771479226</v>
+        <v>5.7580667408249635</v>
       </c>
       <c r="P15" s="2">
-        <v>439.58204012214867</v>
+        <v>11.581052118850463</v>
       </c>
       <c r="Q15" s="2">
-        <v>564.083479530575</v>
+        <v>14.611531070603711</v>
       </c>
       <c r="R15" s="2">
-        <v>239.51376191422165</v>
+        <v>17.820791487236153</v>
       </c>
       <c r="S15" s="2">
-        <v>1123.7866460773278</v>
+        <v>12.257351084779426</v>
       </c>
       <c r="T15" s="2">
-        <v>767.03902544862467</v>
+        <v>2.3208394422467289</v>
       </c>
       <c r="U15" s="2">
-        <v>658.30929979750329</v>
+        <v>5.6405288451247895</v>
       </c>
       <c r="V15" s="2">
-        <v>947.71971898363927</v>
+        <v>5.6792070214869437</v>
       </c>
       <c r="W15" s="2">
-        <v>1054.3778000746013</v>
-      </c>
-      <c r="X15" s="2">
-        <v>654.78254149509212</v>
-      </c>
-      <c r="Y15" s="8">
-        <v>146.68825817225766</v>
-      </c>
-      <c r="Z15" s="2">
-        <v>486.38571052949459</v>
-      </c>
-      <c r="AA15" s="2">
-        <v>468.26359991557382</v>
-      </c>
-      <c r="AB15" s="2">
-        <v>527.42296273292084</v>
-      </c>
+        <v>5.241076318480606</v>
+      </c>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="6">
         <v>2019</v>
       </c>
       <c r="B16" s="2">
-        <v>524.45000122616625</v>
+        <v>5.0732958205879646</v>
       </c>
       <c r="C16" s="2">
-        <v>698.36992889870078</v>
+        <v>7.9535151228248502</v>
       </c>
       <c r="D16" s="2">
-        <v>791.70595096781278</v>
+        <v>4.4872764618581717</v>
       </c>
       <c r="E16" s="2">
-        <v>771.32099128836865</v>
+        <v>8.4534460492244179</v>
       </c>
       <c r="F16" s="2">
-        <v>706.77633573378523</v>
+        <v>8.1992070984403735</v>
       </c>
       <c r="G16" s="2">
-        <v>734.81197833437568</v>
+        <v>7.8326053292672864</v>
       </c>
       <c r="H16" s="2">
-        <v>717.79742848254307</v>
+        <v>6.233265880261933</v>
       </c>
       <c r="I16" s="2">
-        <v>649.41277269999716</v>
+        <v>10.712355474754697</v>
       </c>
       <c r="J16" s="2">
-        <v>580.82248101708467</v>
+        <v>10.211076476411373</v>
       </c>
       <c r="K16" s="2">
-        <v>652.73658243728039</v>
+        <v>2.3603975944650815</v>
       </c>
       <c r="L16" s="2">
-        <v>267.10737214826622</v>
+        <v>1.3028866482684192</v>
       </c>
       <c r="M16" s="2">
-        <v>619.88411827425693</v>
+        <v>7.0333420316024462</v>
       </c>
       <c r="N16" s="2">
-        <v>350.29407594510519</v>
+        <v>5.3672174603893072</v>
       </c>
       <c r="O16" s="2">
-        <v>626.31115071283091</v>
+        <v>5.8312852471864902</v>
       </c>
       <c r="P16" s="2">
-        <v>463.6760627833695</v>
+        <v>11.154067575638624</v>
       </c>
       <c r="Q16" s="2">
-        <v>621.30791443004159</v>
+        <v>9.8083955071280737</v>
       </c>
       <c r="R16" s="2">
-        <v>224.86991801916167</v>
+        <v>17.88498659530724</v>
       </c>
       <c r="S16" s="2">
-        <v>1095.4327344259971</v>
+        <v>10.813108147311652</v>
       </c>
       <c r="T16" s="2">
-        <v>855.6014305590503</v>
+        <v>2.6376672558086782</v>
       </c>
       <c r="U16" s="2">
-        <v>732.76307630757356</v>
+        <v>5.7234369093230857</v>
       </c>
       <c r="V16" s="2">
-        <v>1008.1750017811886</v>
+        <v>5.7426686555903377</v>
       </c>
       <c r="W16" s="2">
-        <v>1067.8786305082633</v>
-      </c>
-      <c r="X16" s="2">
-        <v>743.54990564095522</v>
-      </c>
-      <c r="Y16" s="2">
-        <v>187.81998760761522</v>
-      </c>
-      <c r="Z16" s="2">
-        <v>534.59890759539394</v>
-      </c>
-      <c r="AA16" s="2">
-        <v>485.07853991316301</v>
-      </c>
-      <c r="AB16" s="2">
-        <v>653.93541653651164</v>
-      </c>
+        <v>5.5539228688730322</v>
+      </c>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
     </row>
     <row r="17" spans="1:28">
       <c r="A17" s="6">
         <v>2020</v>
       </c>
       <c r="B17" s="2">
-        <v>584.53423376604258</v>
+        <v>7.4608719196428535</v>
       </c>
       <c r="C17" s="2">
-        <v>697.78191945804849</v>
+        <v>11.039653349977163</v>
       </c>
       <c r="D17" s="2">
-        <v>698.91303104524377</v>
+        <v>5.2860279532464389</v>
       </c>
       <c r="E17" s="2">
-        <v>678.40875429780476</v>
+        <v>10.722801290579092</v>
       </c>
       <c r="F17" s="2">
-        <v>783.80331823815118</v>
+        <v>12.169081893467469</v>
       </c>
       <c r="G17" s="2">
-        <v>743.19835054004784</v>
+        <v>10.521758215010252</v>
       </c>
       <c r="H17" s="2">
-        <v>603.46486949997325</v>
+        <v>8.5192567517127991</v>
       </c>
       <c r="I17" s="2">
-        <v>583.2099092243883</v>
+        <v>11.088901069228374</v>
       </c>
       <c r="J17" s="2">
-        <v>580.8322199083143</v>
+        <v>16.417178644900766</v>
       </c>
       <c r="K17" s="2">
-        <v>658.90962547881895</v>
+        <v>3.6287874289999658</v>
       </c>
       <c r="L17" s="2">
-        <v>313.87762847450199</v>
+        <v>2.281288985231269</v>
       </c>
       <c r="M17" s="2">
-        <v>657.51939083301204</v>
+        <v>15.744711152627222</v>
       </c>
       <c r="N17" s="2">
-        <v>391.42857282535897</v>
+        <v>10.749929971177812</v>
       </c>
       <c r="O17" s="2">
-        <v>574.74307529514283</v>
+        <v>7.9479637005397583</v>
       </c>
       <c r="P17" s="2">
-        <v>466.90212575781129</v>
+        <v>17.97320953102529</v>
       </c>
       <c r="Q17" s="2">
-        <v>584.25262321184323</v>
+        <v>11.984034776251665</v>
       </c>
       <c r="R17" s="2">
-        <v>338.2069281600667</v>
+        <v>21.062868237194383</v>
       </c>
       <c r="S17" s="2">
-        <v>714.91844728099318</v>
+        <v>17.704577081620283</v>
       </c>
       <c r="T17" s="2">
-        <v>841.4338684253953</v>
+        <v>3.6448415753059855</v>
       </c>
       <c r="U17" s="2">
-        <v>707.30975471209013</v>
+        <v>7.9850354421049214</v>
       </c>
       <c r="V17" s="2">
-        <v>807.54622140484548</v>
+        <v>8.1491778101014738</v>
       </c>
       <c r="W17" s="2">
-        <v>1228.2989913764206</v>
-      </c>
-      <c r="X17" s="2">
-        <v>557.11907172338601</v>
-      </c>
-      <c r="Y17" s="2">
-        <v>282.18903071174589</v>
-      </c>
-      <c r="Z17" s="2">
-        <v>583.15888728740606</v>
-      </c>
-      <c r="AA17" s="2">
-        <v>550.78714252684972</v>
-      </c>
-      <c r="AB17" s="2">
-        <v>698.45273767717322</v>
-      </c>
+        <v>5.4748676859231846</v>
+      </c>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
     </row>
     <row r="18" spans="1:28">
       <c r="A18" s="6">
         <v>2021</v>
       </c>
       <c r="B18" s="2">
-        <v>671.50360851082496</v>
+        <v>10.159848978137999</v>
       </c>
       <c r="C18" s="2">
-        <v>752.22325551276003</v>
+        <v>11.377150225792001</v>
       </c>
       <c r="D18" s="2">
-        <v>798.87990342194996</v>
+        <v>6.2110770091565097</v>
       </c>
       <c r="E18" s="2">
-        <v>819.54132047889004</v>
+        <v>9.7138529341875408</v>
       </c>
       <c r="F18" s="2">
-        <v>844.354137865903</v>
+        <v>14.034929751070701</v>
       </c>
       <c r="G18" s="2">
-        <v>771.65355659126305</v>
+        <v>11.0197064251073</v>
       </c>
       <c r="H18" s="2">
-        <v>726.79804899193402</v>
+        <v>6.9692125435529304</v>
       </c>
       <c r="I18" s="2">
-        <v>651.21854082187599</v>
+        <v>14.311459383789799</v>
       </c>
       <c r="J18" s="2">
-        <v>571.448489112522</v>
+        <v>14.903506740585399</v>
       </c>
       <c r="K18" s="2">
-        <v>706.82822059230705</v>
+        <v>7.3242297142988102</v>
       </c>
       <c r="L18" s="2">
-        <v>456.51578120233398</v>
+        <v>4.4260164185606197</v>
       </c>
       <c r="M18" s="2">
-        <v>751.73936891018502</v>
+        <v>11.3514220726414</v>
       </c>
       <c r="N18" s="2">
-        <v>480.90014471204501</v>
+        <v>10.9223800666368</v>
       </c>
       <c r="O18" s="2">
-        <v>651.67586499459401</v>
+        <v>13.1439035660384</v>
       </c>
       <c r="P18" s="2">
-        <v>526.57962001840099</v>
+        <v>23.1243482204857</v>
       </c>
       <c r="Q18" s="2">
-        <v>770.59008546273503</v>
+        <v>18.518410779467501</v>
       </c>
       <c r="R18" s="2">
-        <v>358.49112417740997</v>
+        <v>25.8715925261357</v>
       </c>
       <c r="S18" s="2">
-        <v>1060.7424534593599</v>
+        <v>17.137813674600199</v>
       </c>
       <c r="T18" s="2">
-        <v>879.59443748761805</v>
+        <v>5.8012715957612002</v>
       </c>
       <c r="U18" s="2">
-        <v>921.24772257821803</v>
+        <v>11.829011033051097</v>
       </c>
       <c r="V18" s="2">
-        <v>1505.3970196661901</v>
+        <v>12.3826033678365</v>
       </c>
       <c r="W18" s="2">
-        <v>1438.1898822870401</v>
-      </c>
-      <c r="X18" s="2">
-        <v>958.33188005989098</v>
-      </c>
-      <c r="Y18" s="2">
-        <v>322.03966524407002</v>
-      </c>
-      <c r="Z18" s="2">
-        <v>688.877023819849</v>
-      </c>
-      <c r="AA18" s="2">
-        <v>645.28688761540104</v>
-      </c>
-      <c r="AB18" s="2">
-        <v>815.311709866206</v>
-      </c>
+        <v>6.10692001795503</v>
+      </c>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
     </row>
     <row r="19" spans="1:28">
       <c r="A19" s="6">
         <v>2022</v>
       </c>
-      <c r="B19" s="2">
-        <v>588.74080638089004</v>
-      </c>
-      <c r="C19" s="2">
-        <v>694.969705691831</v>
-      </c>
-      <c r="D19" s="2">
-        <v>741.18959294184401</v>
-      </c>
-      <c r="E19" s="2">
-        <v>717.23817183395795</v>
-      </c>
-      <c r="F19" s="2">
-        <v>726.576911051607</v>
-      </c>
-      <c r="G19" s="2">
-        <v>748.05682893476205</v>
-      </c>
-      <c r="H19" s="2">
-        <v>617.95689795843998</v>
-      </c>
-      <c r="I19" s="2">
-        <v>655.74884434315697</v>
-      </c>
-      <c r="J19" s="2">
-        <v>542.91632880686097</v>
-      </c>
-      <c r="K19" s="2">
-        <v>632.278737080479</v>
-      </c>
-      <c r="L19" s="2">
-        <v>362.36226490528998</v>
-      </c>
-      <c r="M19" s="2">
-        <v>592.89910081457299</v>
-      </c>
-      <c r="N19" s="2">
-        <v>411.38436799619399</v>
-      </c>
-      <c r="O19" s="2">
-        <v>674.957233923064</v>
-      </c>
-      <c r="P19" s="2">
-        <v>575.03585814746202</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>668.95055036297401</v>
-      </c>
-      <c r="R19" s="2">
-        <v>329.72437821375399</v>
-      </c>
-      <c r="S19" s="2">
-        <v>1430.19241324779</v>
-      </c>
-      <c r="T19" s="2">
-        <v>879.99700292725197</v>
-      </c>
-      <c r="U19" s="2">
-        <v>697.19800818643705</v>
-      </c>
-      <c r="V19" s="2">
-        <v>1102.4247872984599</v>
-      </c>
-      <c r="W19" s="2">
-        <v>1267.19374137613</v>
-      </c>
-      <c r="X19" s="2">
-        <v>1146.5447929807101</v>
-      </c>
-      <c r="Y19" s="2">
-        <v>205.23645693205401</v>
-      </c>
-      <c r="Z19" s="2">
-        <v>591.65555640774005</v>
-      </c>
-      <c r="AA19" s="2">
-        <v>632.57540534716395</v>
-      </c>
-      <c r="AB19" s="2">
-        <v>486.96447439743503</v>
-      </c>
+      <c r="B19" s="7">
+        <v>6.7038538622680797</v>
+      </c>
+      <c r="C19" s="7">
+        <v>9.1561439245793395</v>
+      </c>
+      <c r="D19" s="7">
+        <v>6.5693529069370502</v>
+      </c>
+      <c r="E19" s="7">
+        <v>6.9082753054426602</v>
+      </c>
+      <c r="F19" s="7">
+        <v>10.5427498573408</v>
+      </c>
+      <c r="G19" s="7">
+        <v>9.2729626065105695</v>
+      </c>
+      <c r="H19" s="7">
+        <v>5.5072983825888597</v>
+      </c>
+      <c r="I19" s="7">
+        <v>14.257595332530901</v>
+      </c>
+      <c r="J19" s="7">
+        <v>12.017839775432099</v>
+      </c>
+      <c r="K19" s="7">
+        <v>3.1762866319237801</v>
+      </c>
+      <c r="L19" s="7">
+        <v>1.5510871260433601</v>
+      </c>
+      <c r="M19" s="7">
+        <v>9.0256306835389797</v>
+      </c>
+      <c r="N19" s="7">
+        <v>13.6348493489295</v>
+      </c>
+      <c r="O19" s="7">
+        <v>6.8686460510318996</v>
+      </c>
+      <c r="P19" s="7">
+        <v>15.9192875025819</v>
+      </c>
+      <c r="Q19" s="7">
+        <v>12.634911930638101</v>
+      </c>
+      <c r="R19" s="7">
+        <v>23.277913279315399</v>
+      </c>
+      <c r="S19" s="7">
+        <v>24.988345522615599</v>
+      </c>
+      <c r="T19" s="7">
+        <v>2.88609874279277</v>
+      </c>
+      <c r="U19" s="7">
+        <v>7.0168567267672</v>
+      </c>
+      <c r="V19" s="7">
+        <v>7.0937558889859202</v>
+      </c>
+      <c r="W19" s="7">
+        <v>6.4043610207341803</v>
+      </c>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
     </row>
     <row r="20" spans="1:28">
       <c r="A20" s="4"/>
@@ -3442,14 +3250,14 @@
     <CEID xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239" xsi:nil="true"/>
     <ContentDate xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">2022-12-30T22:00:00+00:00</ContentDate>
     <ShowInContentGroups xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239"/>
-    <ParentDataSet xmlns="6152e2e9-49a3-491d-83d0-b758bddb6f14">42</ParentDataSet>
+    <ParentDataSet xmlns="6152e2e9-49a3-491d-83d0-b758bddb6f14">46</ParentDataSet>
     <Order0 xmlns="6152e2e9-49a3-491d-83d0-b758bddb6f14">2022123100</Order0>
     <PublicationDate xmlns="6152e2e9-49a3-491d-83d0-b758bddb6f14">2023-03-30T21:00:00+00:00</PublicationDate>
     <Description0 xmlns="6152e2e9-49a3-491d-83d0-b758bddb6f14" xsi:nil="true"/>
     <AModifiedBy xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">System Account</AModifiedBy>
-    <AModified xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">2023-03-30T20:40:17+00:00</AModified>
-    <AID xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">7377</AID>
-    <ACreated xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">2023-03-24T13:54:43+00:00</ACreated>
+    <AModified xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">2023-03-30T20:38:56+00:00</AModified>
+    <AID xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">7369</AID>
+    <ACreated xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">2023-03-24T13:54:45+00:00</ACreated>
     <ACreatedBy xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">Moutti Maria</ACreatedBy>
     <AVersion xmlns="a029a951-197a-4454-90a0-4e8ba8bb2239">1.0</AVersion>
   </documentManagement>
@@ -3457,13 +3265,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{425094FC-6392-4A6C-9FEE-065A6A1C2654}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F1CD883-7C68-4FF4-BB21-F67B3B7F7C0F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B97D9FF7-C70A-40C0-BD23-ACE69BCB8F49}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B51C0A9-4E0E-4431-9146-0E5A966EF578}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FAFA469-A1CE-4AB1-9B4E-C48C506D121D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA950F2-842B-4042-9031-8BBE9D4F0702}"/>
 </file>
</xml_diff>